<commit_message>
Adding Lizzie and Cat's handwritten notes from planting day
... as best I could
</commit_message>
<xml_diff>
--- a/Planning/planning_2018/Planted_2018.xlsx
+++ b/Planning/planning_2018/Planted_2018.xlsx
@@ -1,34 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/wildhellgarden/Planning/planning_2018/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="27920" yWindow="1560" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>IND</t>
   </si>
@@ -151,13 +146,73 @@
   </si>
   <si>
     <t>BETALL09_WM</t>
+  </si>
+  <si>
+    <t>File started in 25 May 2018 by Cat Chamberlain</t>
+  </si>
+  <si>
+    <t>Column info (by Cat):</t>
+  </si>
+  <si>
+    <t>More metadata (by Lizzie):</t>
+  </si>
+  <si>
+    <t>Planting took place on 14 May 2018 by Kea Woodruff, Cat C., Dan B. and Lizzie</t>
+  </si>
+  <si>
+    <t>We worked off the notes: planningnotes_2018 and planningnotes_2018_updatebyemail and mostly a paper list that Cat had, according to that list we:</t>
+  </si>
+  <si>
+    <t>Replaced:</t>
+  </si>
+  <si>
+    <t>One mislabeled ALNINC WM in plot 3 (and left what was there)</t>
+  </si>
+  <si>
+    <t>Recoverable 1 AROMEL WM (perhaps in plot 4)</t>
+  </si>
+  <si>
+    <t>Recoverable 2 BETALL (1 GR, 1 SH -- probably plots 9 and 15)</t>
+  </si>
+  <si>
+    <t>Recoverable DIELON (not sure how many, plot 10 probably)</t>
+  </si>
+  <si>
+    <t>Recoverable 1 SORAME</t>
+  </si>
+  <si>
+    <t>Backups:</t>
+  </si>
+  <si>
+    <t>4 ALNINC (HF, WM, SH, GR)</t>
+  </si>
+  <si>
+    <t>2 BETPOP (GR, WM)</t>
+  </si>
+  <si>
+    <t>3 VIBCAS (WM, GR, SH)</t>
+  </si>
+  <si>
+    <t>2 AROMEL (HF, WM)</t>
+  </si>
+  <si>
+    <t>3 BETALL (WM, GR, SH)</t>
+  </si>
+  <si>
+    <t>2 MYRGAL (WM, SH … did not find a GR to add)</t>
+  </si>
+  <si>
+    <t>Cat worked up the data in data tab 10 days after planting, she wrote: I was able to quickly make a new excel file with all of the plants we planted a couple of weeks ago. The third column is `From CG or RB?' which is saying whether or not we moved it from another CG plot or moved it from the RB.</t>
+  </si>
+  <si>
+    <t>I scratched some hideous notes of things we added in as we found them in the RB (most of these are replacements for what was lost), these notes are not so great, looks like BETPAP, SPIALB, SPITOM, DIELON, SORAME, and some VACMYR were also added in. See the data tab for the final tally.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -168,6 +223,37 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -189,14 +275,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -252,7 +360,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -287,7 +395,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -464,7 +572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -475,12 +583,15 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -502,7 +613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -513,7 +624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -524,7 +635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -535,7 +646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -546,7 +657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -557,7 +668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -568,7 +679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -579,7 +690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -590,7 +701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -601,7 +712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -612,7 +723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -623,7 +734,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -634,7 +745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -645,7 +756,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -656,7 +767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -667,7 +778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -678,7 +789,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -689,7 +800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -700,7 +811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -711,7 +822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -722,7 +833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -733,7 +844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -744,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -755,7 +866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -766,7 +877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -777,7 +888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -788,7 +899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -799,7 +910,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -810,7 +921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -821,7 +932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
         <v>20</v>
       </c>
@@ -832,7 +943,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
@@ -843,7 +954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
@@ -854,7 +965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -865,7 +976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
@@ -876,7 +987,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
@@ -887,7 +998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
@@ -898,7 +1009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -909,7 +1020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -920,7 +1031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -931,7 +1042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -944,28 +1055,135 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>